<commit_message>
pws multiple calculation for t values
</commit_message>
<xml_diff>
--- a/performance_test/SIGN.xlsx
+++ b/performance_test/SIGN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\Thesis\DBV-ISP\DBV-ISP-Miner\performance_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2344A189-36F4-45FC-B07E-43B2F9AECF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DB7E5F-9A7F-4291-A80E-89C98D5AF4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3165" yWindow="1560" windowWidth="12765" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,13 +115,13 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -407,7 +407,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,16 +420,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -466,161 +466,163 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>2401</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="E5" s="3">
+      <c r="C5" s="1"/>
+      <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>676</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="I5" s="3">
+      <c r="G5" s="1"/>
+      <c r="I5" s="1">
         <v>1</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>624</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3">
+      <c r="C6" s="1"/>
+      <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>263</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="I6" s="3">
+      <c r="G6" s="1"/>
+      <c r="I6" s="1">
         <v>2</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>1758</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3">
+      <c r="C7" s="1">
+        <v>8320</v>
+      </c>
+      <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>524</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="1">
         <v>312.85300000000001</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="1">
         <v>3</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>1629</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="E8" s="3">
+      <c r="C8" s="1"/>
+      <c r="E8" s="1">
         <v>4</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>242</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="I8" s="3">
+      <c r="G8" s="1"/>
+      <c r="I8" s="1">
         <v>4</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>547</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="E9" s="3">
+      <c r="C9" s="1"/>
+      <c r="E9" s="1">
         <v>5</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="1">
         <v>26</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3">
+      <c r="G9" s="1"/>
+      <c r="I9" s="1">
         <v>5</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>45</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="E10" s="3">
+      <c r="C10" s="1"/>
+      <c r="E10" s="1">
         <v>6</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="I10" s="3">
+      <c r="G10" s="1"/>
+      <c r="I10" s="1">
         <v>6</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>